<commit_message>
Etapa 3 kmedias lista
</commit_message>
<xml_diff>
--- a/esquema de reglas corregido.xlsx
+++ b/esquema de reglas corregido.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7680" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7680" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Entendimiento del negcio" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="185">
   <si>
     <t>Procedimiento</t>
   </si>
@@ -576,6 +576,12 @@
   </si>
   <si>
     <t>Inicie el algoritmo, si desea hacerlo mediante la evaluacion de una clase seleccione una clase nominal en la barra de "Classes to cluster evaluation" si desea hacerlo eliminando una parte de los datos seleccione "percentage split" e ingrese como valor 70%</t>
+  </si>
+  <si>
+    <t>EliminarValoresAnomalosYValoresExtremos</t>
+  </si>
+  <si>
+    <t>finEtapa</t>
   </si>
 </sst>
 </file>
@@ -619,7 +625,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -679,11 +685,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -750,44 +769,44 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -797,6 +816,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1111,13 +1139,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24">
+      <c r="A2" s="25">
         <v>1</v>
       </c>
-      <c r="B2" s="24">
+      <c r="B2" s="25">
         <v>1</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="25" t="s">
         <v>60</v>
       </c>
       <c r="D2" s="10" t="s">
@@ -1128,31 +1156,31 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="24" t="s">
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="25" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="0.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
     </row>
     <row r="5" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="25" t="s">
         <v>78</v>
       </c>
       <c r="D5" s="10" t="s">
@@ -1163,9 +1191,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
       <c r="D6" s="10" t="s">
         <v>5</v>
       </c>
@@ -1174,13 +1202,13 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="25" t="s">
         <v>61</v>
       </c>
       <c r="D7" s="10" t="s">
@@ -1191,9 +1219,9 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
       <c r="D8" s="10" t="s">
         <v>5</v>
       </c>
@@ -1202,13 +1230,13 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="24">
+      <c r="B9" s="25">
         <v>2</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="25" t="s">
         <v>53</v>
       </c>
       <c r="D9" s="11" t="s">
@@ -1219,9 +1247,9 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
       <c r="D10" s="26" t="s">
         <v>5</v>
       </c>
@@ -1230,22 +1258,22 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
       <c r="D11" s="26"/>
       <c r="E11" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="25" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="11" t="s">
@@ -1256,9 +1284,9 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
       <c r="D13" s="11" t="s">
         <v>5</v>
       </c>
@@ -1267,13 +1295,13 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="25" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="11" t="s">
@@ -1284,9 +1312,9 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
       <c r="D15" s="26" t="s">
         <v>5</v>
       </c>
@@ -1295,22 +1323,22 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
       <c r="D16" s="26"/>
       <c r="E16" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="25" t="s">
         <v>41</v>
       </c>
       <c r="D17" s="11" t="s">
@@ -1321,9 +1349,9 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
       <c r="D18" s="26" t="s">
         <v>5</v>
       </c>
@@ -1332,9 +1360,9 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
       <c r="D19" s="26"/>
       <c r="E19" s="10" t="s">
         <v>21</v>
@@ -1358,13 +1386,13 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="24">
+      <c r="B21" s="25">
         <v>3</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="25" t="s">
         <v>62</v>
       </c>
       <c r="D21" s="11" t="s">
@@ -1375,9 +1403,9 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
       <c r="D22" s="26" t="s">
         <v>5</v>
       </c>
@@ -1386,22 +1414,22 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="24"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
       <c r="D23" s="26"/>
       <c r="E23" s="10" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="25" t="s">
         <v>63</v>
       </c>
       <c r="D24" s="10" t="s">
@@ -1412,9 +1440,9 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="24"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
       <c r="D25" s="10" t="s">
         <v>5</v>
       </c>
@@ -1423,13 +1451,13 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="24" t="s">
+      <c r="A26" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="24">
-        <v>4</v>
-      </c>
-      <c r="C26" s="24" t="s">
+      <c r="B26" s="25">
+        <v>4</v>
+      </c>
+      <c r="C26" s="25" t="s">
         <v>64</v>
       </c>
       <c r="D26" s="10" t="s">
@@ -1440,31 +1468,31 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="24"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="24" t="s">
+      <c r="A27" s="25"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="25" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="24"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
     </row>
     <row r="29" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="C29" s="25" t="s">
         <v>66</v>
       </c>
       <c r="D29" s="10" t="s">
@@ -1475,9 +1503,9 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="24"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
+      <c r="A30" s="25"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
       <c r="D30" s="10" t="s">
         <v>5</v>
       </c>
@@ -1486,13 +1514,13 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="24">
-        <v>5</v>
-      </c>
-      <c r="C31" s="24" t="s">
+      <c r="B31" s="25">
+        <v>5</v>
+      </c>
+      <c r="C31" s="25" t="s">
         <v>69</v>
       </c>
       <c r="D31" s="11" t="s">
@@ -1503,38 +1531,38 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="24"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="24"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
       <c r="D32" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E32" s="24" t="s">
+      <c r="E32" s="25" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="24"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
+      <c r="A33" s="25"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
       <c r="D33" s="26"/>
-      <c r="E33" s="24"/>
+      <c r="E33" s="25"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="24"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
       <c r="D34" s="26"/>
-      <c r="E34" s="24"/>
+      <c r="E34" s="25"/>
     </row>
     <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="24" t="s">
+      <c r="A35" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="B35" s="24" t="s">
+      <c r="B35" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="24" t="s">
+      <c r="C35" s="25" t="s">
         <v>70</v>
       </c>
       <c r="D35" s="11" t="s">
@@ -1545,9 +1573,9 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="24"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
+      <c r="A36" s="25"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="25"/>
       <c r="D36" s="26" t="s">
         <v>5</v>
       </c>
@@ -1556,9 +1584,9 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="24"/>
-      <c r="B37" s="24"/>
-      <c r="C37" s="24"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
       <c r="D37" s="26"/>
       <c r="E37" s="10" t="s">
         <v>29</v>
@@ -1582,13 +1610,13 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="28" t="s">
+      <c r="A39" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="25">
+      <c r="B39" s="24">
         <v>6</v>
       </c>
-      <c r="C39" s="25" t="s">
+      <c r="C39" s="24" t="s">
         <v>77</v>
       </c>
       <c r="D39" s="13" t="s">
@@ -1599,10 +1627,10 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="29"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="27" t="s">
+      <c r="A40" s="28"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="30" t="s">
         <v>5</v>
       </c>
       <c r="E40" s="14" t="s">
@@ -1610,22 +1638,22 @@
       </c>
     </row>
     <row r="41" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="30"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="27"/>
+      <c r="A41" s="29"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="30"/>
       <c r="E41" s="14" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="B42" s="25" t="s">
+      <c r="B42" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C42" s="25" t="s">
+      <c r="C42" s="24" t="s">
         <v>73</v>
       </c>
       <c r="D42" s="14" t="s">
@@ -1636,9 +1664,9 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="25"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
+      <c r="A43" s="24"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="24"/>
       <c r="D43" s="14" t="s">
         <v>5</v>
       </c>
@@ -1647,13 +1675,13 @@
       </c>
     </row>
     <row r="44" spans="1:5" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="25" t="s">
+      <c r="A44" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="25">
+      <c r="B44" s="24">
         <v>7</v>
       </c>
-      <c r="C44" s="25" t="s">
+      <c r="C44" s="24" t="s">
         <v>55</v>
       </c>
       <c r="D44" s="14" t="s">
@@ -1664,9 +1692,9 @@
       </c>
     </row>
     <row r="45" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="25"/>
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
+      <c r="A45" s="24"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="24"/>
       <c r="D45" s="14" t="s">
         <v>36</v>
       </c>
@@ -1675,13 +1703,13 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="25" t="s">
+      <c r="A46" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="25">
+      <c r="B46" s="24">
         <v>8</v>
       </c>
-      <c r="C46" s="25" t="s">
+      <c r="C46" s="24" t="s">
         <v>56</v>
       </c>
       <c r="D46" s="14" t="s">
@@ -1692,9 +1720,9 @@
       </c>
     </row>
     <row r="47" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="25"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="25"/>
+      <c r="A47" s="24"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="24"/>
       <c r="D47" s="14" t="s">
         <v>36</v>
       </c>
@@ -1703,13 +1731,13 @@
       </c>
     </row>
     <row r="48" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="25" t="s">
+      <c r="A48" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="B48" s="25">
+      <c r="B48" s="24">
         <v>9</v>
       </c>
-      <c r="C48" s="25" t="s">
+      <c r="C48" s="24" t="s">
         <v>37</v>
       </c>
       <c r="D48" s="14" t="s">
@@ -1720,9 +1748,9 @@
       </c>
     </row>
     <row r="49" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="25"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
+      <c r="A49" s="24"/>
+      <c r="B49" s="24"/>
+      <c r="C49" s="24"/>
       <c r="D49" s="13" t="s">
         <v>36</v>
       </c>
@@ -1731,13 +1759,13 @@
       </c>
     </row>
     <row r="50" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="25" t="s">
+      <c r="A50" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="B50" s="25">
+      <c r="B50" s="24">
         <v>10</v>
       </c>
-      <c r="C50" s="25" t="s">
+      <c r="C50" s="24" t="s">
         <v>165</v>
       </c>
       <c r="D50" s="13" t="s">
@@ -1748,9 +1776,9 @@
       </c>
     </row>
     <row r="51" spans="1:5" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="25"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="25"/>
+      <c r="A51" s="24"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="24"/>
       <c r="D51" s="13" t="s">
         <v>5</v>
       </c>
@@ -1759,30 +1787,30 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="25"/>
-      <c r="B52" s="25"/>
-      <c r="C52" s="25"/>
+      <c r="A52" s="24"/>
+      <c r="B52" s="24"/>
+      <c r="C52" s="24"/>
       <c r="D52" s="13"/>
       <c r="E52" s="14"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="25"/>
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
+      <c r="A53" s="24"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="24"/>
       <c r="D53" s="13"/>
       <c r="E53" s="13"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="24"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="24"/>
+      <c r="A54" s="25"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="25"/>
       <c r="D54" s="11"/>
       <c r="E54" s="10"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="24"/>
-      <c r="B55" s="24"/>
-      <c r="C55" s="24"/>
+      <c r="A55" s="25"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="25"/>
       <c r="D55" s="11"/>
       <c r="E55" s="10"/>
     </row>
@@ -1795,35 +1823,36 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="E32:E34"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D27:D28"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
@@ -1840,36 +1869,35 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="C9:C11"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="D32:D34"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="E32:E34"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A39:A41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1918,16 +1946,16 @@
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="34">
+      <c r="B2" s="33">
         <v>1</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="33" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="16" t="s">
@@ -1935,27 +1963,27 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
       <c r="E3" s="16" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
       <c r="E4" s="16" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
       <c r="D5" s="16" t="s">
         <v>4</v>
       </c>
@@ -1996,16 +2024,16 @@
       <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:12" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="B8" s="33">
+      <c r="B8" s="34">
         <v>2</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="16" t="s">
@@ -2014,18 +2042,18 @@
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
+      <c r="A9" s="34"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
       <c r="E9" s="17">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="17" t="s">
         <v>5</v>
       </c>
@@ -2035,16 +2063,16 @@
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:12" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E11" s="21" t="s">
@@ -2053,18 +2081,18 @@
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="33"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
       <c r="E12" s="17">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="33"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
       <c r="D13" s="17" t="s">
         <v>5</v>
       </c>
@@ -2073,13 +2101,13 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="33" t="s">
         <v>89</v>
       </c>
       <c r="D14" s="17" t="s">
@@ -2090,9 +2118,9 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="33"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="34"/>
+      <c r="A15" s="34"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="33"/>
       <c r="D15" s="17" t="s">
         <v>5</v>
       </c>
@@ -2101,16 +2129,16 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="B16" s="33">
+      <c r="B16" s="34">
         <v>3</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="D16" s="33" t="s">
+      <c r="D16" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E16" s="17" t="s">
@@ -2118,76 +2146,76 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="34"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="33"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="34"/>
       <c r="E17" s="17" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="33"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="34"/>
       <c r="E18" s="17" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="34"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="33"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="34"/>
       <c r="E19" s="17" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="34"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="33"/>
+      <c r="A20" s="33"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="34"/>
       <c r="E20" s="17" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="34"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="33"/>
+      <c r="A21" s="33"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="34"/>
       <c r="E21" s="17" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="33"/>
+      <c r="A22" s="33"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="34"/>
       <c r="E22" s="17">
         <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="34"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" s="33" t="s">
+      <c r="A23" s="33"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="34" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="34"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
+      <c r="A24" s="33"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
@@ -2207,16 +2235,16 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="36" t="s">
         <v>103</v>
       </c>
       <c r="B26" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="32" t="s">
+      <c r="C26" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="D26" s="32" t="s">
+      <c r="D26" s="36" t="s">
         <v>4</v>
       </c>
       <c r="E26" s="20" t="s">
@@ -2224,37 +2252,37 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A27" s="32"/>
+      <c r="A27" s="36"/>
       <c r="B27" s="31"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
       <c r="E27" s="20" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="32"/>
+      <c r="A28" s="36"/>
       <c r="B28" s="31"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
       <c r="E28" s="20" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="68.25" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
+      <c r="A29" s="36"/>
       <c r="B29" s="31"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
       <c r="E29" s="20" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="32"/>
+      <c r="A30" s="36"/>
       <c r="B30" s="31"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
       <c r="E30" s="20">
         <v>4</v>
       </c>
@@ -2272,7 +2300,7 @@
       <c r="D31" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="E31" s="32" t="s">
+      <c r="E31" s="36" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2281,7 +2309,7 @@
       <c r="B32" s="31"/>
       <c r="C32" s="31"/>
       <c r="D32" s="31"/>
-      <c r="E32" s="32"/>
+      <c r="E32" s="36"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="31"/>
@@ -2298,13 +2326,13 @@
       <c r="A34" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="B34" s="32">
-        <v>5</v>
-      </c>
-      <c r="C34" s="32" t="s">
+      <c r="B34" s="36">
+        <v>5</v>
+      </c>
+      <c r="C34" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="D34" s="32" t="s">
+      <c r="D34" s="36" t="s">
         <v>5</v>
       </c>
       <c r="E34" s="20" t="s">
@@ -2313,63 +2341,63 @@
     </row>
     <row r="35" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A35" s="31"/>
-      <c r="B35" s="32"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="36"/>
       <c r="E35" s="20" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A36" s="31"/>
-      <c r="B36" s="32"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
       <c r="E36" s="20" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="31"/>
-      <c r="B37" s="32"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="36"/>
       <c r="E37" s="20" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A38" s="31"/>
-      <c r="B38" s="32"/>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
       <c r="E38" s="20" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A39" s="31"/>
-      <c r="B39" s="32"/>
-      <c r="C39" s="32"/>
-      <c r="D39" s="32"/>
+      <c r="B39" s="36"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="36"/>
       <c r="E39" s="20" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="31"/>
-      <c r="B40" s="32"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
       <c r="E40" s="20" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="31"/>
-      <c r="B41" s="32"/>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="36"/>
       <c r="E41" s="20" t="s">
         <v>110</v>
       </c>
@@ -2415,7 +2443,7 @@
       <c r="A45" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="B45" s="36">
+      <c r="B45" s="32">
         <v>1</v>
       </c>
       <c r="C45" s="31" t="s">
@@ -2430,7 +2458,7 @@
     </row>
     <row r="46" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A46" s="31"/>
-      <c r="B46" s="36"/>
+      <c r="B46" s="32"/>
       <c r="C46" s="31"/>
       <c r="D46" s="31"/>
       <c r="E46" s="20" t="s">
@@ -2439,7 +2467,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="31"/>
-      <c r="B47" s="36"/>
+      <c r="B47" s="32"/>
       <c r="C47" s="31"/>
       <c r="D47" s="31"/>
       <c r="E47" s="20" t="s">
@@ -2448,7 +2476,7 @@
     </row>
     <row r="48" spans="1:5" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A48" s="31"/>
-      <c r="B48" s="36"/>
+      <c r="B48" s="32"/>
       <c r="C48" s="31"/>
       <c r="D48" s="31"/>
       <c r="E48" s="20" t="s">
@@ -2457,7 +2485,7 @@
     </row>
     <row r="49" spans="1:5" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A49" s="31"/>
-      <c r="B49" s="36"/>
+      <c r="B49" s="32"/>
       <c r="C49" s="31"/>
       <c r="D49" s="31"/>
       <c r="E49" s="20" t="s">
@@ -2466,7 +2494,7 @@
     </row>
     <row r="50" spans="1:5" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A50" s="31"/>
-      <c r="B50" s="36"/>
+      <c r="B50" s="32"/>
       <c r="C50" s="31"/>
       <c r="D50" s="31"/>
       <c r="E50" s="20" t="s">
@@ -2475,7 +2503,7 @@
     </row>
     <row r="51" spans="1:5" ht="102" x14ac:dyDescent="0.25">
       <c r="A51" s="31"/>
-      <c r="B51" s="36"/>
+      <c r="B51" s="32"/>
       <c r="C51" s="31"/>
       <c r="D51" s="31"/>
       <c r="E51" s="23" t="s">
@@ -2484,7 +2512,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="31"/>
-      <c r="B52" s="36"/>
+      <c r="B52" s="32"/>
       <c r="C52" s="31"/>
       <c r="D52" s="31" t="s">
         <v>181</v>
@@ -2495,7 +2523,7 @@
     </row>
     <row r="53" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A53" s="31"/>
-      <c r="B53" s="36"/>
+      <c r="B53" s="32"/>
       <c r="C53" s="31"/>
       <c r="D53" s="31"/>
       <c r="E53" s="20" t="s">
@@ -2504,7 +2532,7 @@
     </row>
     <row r="54" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A54" s="31"/>
-      <c r="B54" s="36"/>
+      <c r="B54" s="32"/>
       <c r="C54" s="31"/>
       <c r="D54" s="31"/>
       <c r="E54" s="20" t="s">
@@ -2513,7 +2541,7 @@
     </row>
     <row r="55" spans="1:5" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A55" s="31"/>
-      <c r="B55" s="36"/>
+      <c r="B55" s="32"/>
       <c r="C55" s="31"/>
       <c r="D55" s="31"/>
       <c r="E55" s="20" t="s">
@@ -2522,18 +2550,24 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="D45:D51"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="C45:C55"/>
-    <mergeCell ref="B45:B55"/>
-    <mergeCell ref="A45:A55"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="C34:C41"/>
+    <mergeCell ref="B34:B41"/>
+    <mergeCell ref="D34:D41"/>
+    <mergeCell ref="A34:A41"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="D26:D30"/>
+    <mergeCell ref="C26:C30"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="D16:D22"/>
+    <mergeCell ref="B16:B24"/>
+    <mergeCell ref="C16:C24"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D23:D24"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="C31:C33"/>
@@ -2550,24 +2584,18 @@
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="B26:B30"/>
     <mergeCell ref="A16:A24"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="D16:D22"/>
-    <mergeCell ref="B16:B24"/>
-    <mergeCell ref="C16:C24"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="D26:D30"/>
-    <mergeCell ref="C26:C30"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="C34:C41"/>
-    <mergeCell ref="B34:B41"/>
-    <mergeCell ref="D34:D41"/>
-    <mergeCell ref="A34:A41"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="D45:D51"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="C45:C55"/>
+    <mergeCell ref="B45:B55"/>
+    <mergeCell ref="A45:A55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2575,10 +2603,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:B31"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48:E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2609,13 +2637,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="B2" s="24">
+      <c r="B2" s="25">
         <v>1</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="25" t="s">
         <v>121</v>
       </c>
       <c r="D2" s="10" t="s">
@@ -2626,10 +2654,10 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24" t="s">
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="10" t="s">
@@ -2637,100 +2665,100 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
       <c r="E4" s="10" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
       <c r="E5" s="10" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
       <c r="E6" s="10" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
       <c r="E7" s="10" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
       <c r="E8" s="10" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
       <c r="E9" s="10" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
       <c r="E10" s="10" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
       <c r="E11" s="10" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
       <c r="E12" s="10" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
       <c r="E13" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="B14" s="24">
+      <c r="B14" s="25">
         <v>2</v>
       </c>
       <c r="C14" s="37" t="s">
@@ -2744,10 +2772,10 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="25"/>
       <c r="C15" s="38"/>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="25" t="s">
         <v>5</v>
       </c>
       <c r="E15" s="10" t="s">
@@ -2755,80 +2783,80 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
-      <c r="B16" s="24"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
       <c r="C16" s="38"/>
-      <c r="D16" s="24"/>
+      <c r="D16" s="25"/>
       <c r="E16" s="10" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
-      <c r="B17" s="24"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="25"/>
       <c r="C17" s="38"/>
-      <c r="D17" s="24"/>
+      <c r="D17" s="25"/>
       <c r="E17" s="10" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
-      <c r="B18" s="24"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="25"/>
       <c r="C18" s="38"/>
-      <c r="D18" s="24"/>
+      <c r="D18" s="25"/>
       <c r="E18" s="10" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
-      <c r="B19" s="24"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="25"/>
       <c r="C19" s="38"/>
-      <c r="D19" s="24"/>
+      <c r="D19" s="25"/>
       <c r="E19" s="10" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
-      <c r="B20" s="24"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="25"/>
       <c r="C20" s="38"/>
-      <c r="D20" s="24"/>
+      <c r="D20" s="25"/>
       <c r="E20" s="10" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="24"/>
-      <c r="B21" s="24"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="25"/>
       <c r="C21" s="38"/>
-      <c r="D21" s="24"/>
+      <c r="D21" s="25"/>
       <c r="E21" s="10" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
-      <c r="B22" s="24"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="25"/>
       <c r="C22" s="38"/>
-      <c r="D22" s="24"/>
+      <c r="D22" s="25"/>
       <c r="E22" s="10" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="24"/>
-      <c r="B23" s="24"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="25"/>
       <c r="C23" s="39"/>
-      <c r="D23" s="24"/>
+      <c r="D23" s="25"/>
       <c r="E23" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="24" t="s">
-        <v>147</v>
+      <c r="A24" s="25" t="s">
+        <v>183</v>
       </c>
       <c r="B24" s="37" t="s">
         <v>11</v>
@@ -2844,10 +2872,10 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="24"/>
+      <c r="A25" s="25"/>
       <c r="B25" s="38"/>
       <c r="C25" s="38"/>
-      <c r="D25" s="24" t="s">
+      <c r="D25" s="25" t="s">
         <v>4</v>
       </c>
       <c r="E25" s="10" t="s">
@@ -2855,55 +2883,55 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="24"/>
+      <c r="A26" s="25"/>
       <c r="B26" s="38"/>
       <c r="C26" s="38"/>
-      <c r="D26" s="24"/>
+      <c r="D26" s="25"/>
       <c r="E26" s="10" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="24"/>
+      <c r="A27" s="25"/>
       <c r="B27" s="38"/>
       <c r="C27" s="38"/>
-      <c r="D27" s="24"/>
+      <c r="D27" s="25"/>
       <c r="E27" s="10" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="24"/>
+      <c r="A28" s="25"/>
       <c r="B28" s="38"/>
       <c r="C28" s="38"/>
-      <c r="D28" s="24"/>
+      <c r="D28" s="25"/>
       <c r="E28" s="10" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="24"/>
+      <c r="A29" s="25"/>
       <c r="B29" s="38"/>
       <c r="C29" s="38"/>
-      <c r="D29" s="24"/>
+      <c r="D29" s="25"/>
       <c r="E29" s="10" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="24"/>
+      <c r="A30" s="25"/>
       <c r="B30" s="38"/>
       <c r="C30" s="38"/>
-      <c r="D30" s="24"/>
+      <c r="D30" s="25"/>
       <c r="E30" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="24"/>
+      <c r="A31" s="25"/>
       <c r="B31" s="39"/>
       <c r="C31" s="39"/>
-      <c r="D31" s="24"/>
+      <c r="D31" s="25"/>
       <c r="E31" s="10">
         <v>3</v>
       </c>
@@ -2927,13 +2955,13 @@
       <c r="F32" s="6"/>
     </row>
     <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="32" t="s">
+      <c r="A33" s="36" t="s">
         <v>148</v>
       </c>
-      <c r="B33" s="32" t="s">
+      <c r="B33" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="C33" s="32" t="s">
+      <c r="C33" s="36" t="s">
         <v>143</v>
       </c>
       <c r="D33" s="7" t="s">
@@ -2944,10 +2972,10 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="32"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="32" t="s">
+      <c r="A34" s="36"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="36" t="s">
         <v>4</v>
       </c>
       <c r="E34" s="15" t="s">
@@ -2955,155 +2983,159 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="32"/>
-      <c r="B35" s="32"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
+      <c r="A35" s="36"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="36"/>
       <c r="E35" s="15" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A36" s="32"/>
-      <c r="B36" s="32"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
+      <c r="A36" s="36"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
       <c r="E36" s="15" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="32"/>
-      <c r="B37" s="32"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
+      <c r="A37" s="36"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="36"/>
       <c r="E37" s="15" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="45.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="32"/>
-      <c r="B38" s="32"/>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32"/>
+      <c r="A38" s="36"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
       <c r="E38" s="15" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="45.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="32"/>
-      <c r="B39" s="32"/>
-      <c r="C39" s="32"/>
-      <c r="D39" s="32"/>
+      <c r="A39" s="36"/>
+      <c r="B39" s="36"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="36"/>
       <c r="E39" s="15" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="32"/>
-      <c r="B40" s="32"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
+      <c r="A40" s="36"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
       <c r="E40" s="15" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="32"/>
-      <c r="B41" s="32"/>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
+      <c r="A41" s="36"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="36"/>
       <c r="E41" s="15">
         <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="32" t="s">
+      <c r="A42" s="36" t="s">
         <v>149</v>
       </c>
-      <c r="B42" s="32">
+      <c r="B42" s="36">
         <v>3</v>
       </c>
-      <c r="C42" s="32" t="s">
+      <c r="C42" s="36" t="s">
         <v>150</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E42" s="15">
-        <v>4</v>
+      <c r="E42" s="15" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A43" s="32"/>
-      <c r="B43" s="32"/>
-      <c r="C43" s="32"/>
-      <c r="D43" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="E43" s="15" t="s">
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" s="40" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="32"/>
-      <c r="B44" s="32"/>
-      <c r="C44" s="32"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="15" t="s">
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="40" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A45" s="32"/>
-      <c r="B45" s="32"/>
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="15" t="s">
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="36"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="40" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="32"/>
-      <c r="B46" s="32"/>
-      <c r="C46" s="32"/>
-      <c r="D46" s="32"/>
-      <c r="E46" s="15" t="s">
+      <c r="A46" s="36"/>
+      <c r="B46" s="36"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="40" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="45.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="32"/>
-      <c r="B47" s="32"/>
-      <c r="C47" s="32"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="15" t="s">
+      <c r="A47" s="36"/>
+      <c r="B47" s="36"/>
+      <c r="C47" s="36"/>
+      <c r="D47" s="36"/>
+      <c r="E47" s="40" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="32"/>
-      <c r="B48" s="32"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="32"/>
-      <c r="E48" s="31" t="s">
+      <c r="A48" s="36"/>
+      <c r="B48" s="36"/>
+      <c r="C48" s="36"/>
+      <c r="D48" s="36"/>
+      <c r="E48" s="41" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="32"/>
-      <c r="B49" s="32"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
-      <c r="E49" s="31"/>
+    <row r="49" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="36"/>
+      <c r="B49" s="36"/>
+      <c r="C49" s="36"/>
+      <c r="D49" s="36"/>
+      <c r="E49" s="41"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="36"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="36"/>
+      <c r="D50" s="36"/>
+      <c r="E50" s="42" t="s">
+        <v>184</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B42:B49"/>
-    <mergeCell ref="C42:C49"/>
-    <mergeCell ref="D43:D49"/>
-    <mergeCell ref="D15:D23"/>
-    <mergeCell ref="A33:A41"/>
     <mergeCell ref="E48:E49"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
@@ -3119,7 +3151,12 @@
     <mergeCell ref="B33:B41"/>
     <mergeCell ref="D25:D31"/>
     <mergeCell ref="B14:B23"/>
-    <mergeCell ref="A42:A49"/>
+    <mergeCell ref="D15:D23"/>
+    <mergeCell ref="A33:A41"/>
+    <mergeCell ref="D43:D50"/>
+    <mergeCell ref="C42:C50"/>
+    <mergeCell ref="B42:B50"/>
+    <mergeCell ref="A42:A50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3128,10 +3165,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33:C41"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3161,13 +3198,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="32" t="s">
         <v>146</v>
       </c>
-      <c r="B2" s="36">
+      <c r="B2" s="32">
         <v>1</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="32" t="s">
         <v>121</v>
       </c>
       <c r="D2" s="8" t="s">
@@ -3178,10 +3215,10 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="36"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36" t="s">
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="8" t="s">
@@ -3189,103 +3226,103 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
       <c r="E4" s="8" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="36"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
+      <c r="A5" s="32"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
       <c r="E5" s="8" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="36"/>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
+      <c r="A6" s="32"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
       <c r="E6" s="8" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
       <c r="E7" s="8" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="36"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
       <c r="E8" s="8" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="36"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
       <c r="E9" s="8" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="36"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
       <c r="E10" s="8" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="36"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
       <c r="E11" s="8" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="36"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
       <c r="E12" s="8" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="36"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
       <c r="E13" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="B14" s="36">
+      <c r="B14" s="32">
         <v>2</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="32" t="s">
         <v>129</v>
       </c>
       <c r="D14" s="8" t="s">
@@ -3296,10 +3333,10 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="36"/>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36" t="s">
+      <c r="A15" s="32"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32" t="s">
         <v>5</v>
       </c>
       <c r="E15" s="8" t="s">
@@ -3307,73 +3344,73 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="36"/>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
       <c r="E16" s="8" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="36"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
       <c r="E17" s="8" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="36"/>
-      <c r="B18" s="36"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
       <c r="E18" s="8" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
       <c r="E19" s="8" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="36"/>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
       <c r="E20" s="8" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="36"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
       <c r="E21" s="8" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="36"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
       <c r="E22" s="8" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="36"/>
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
+      <c r="A23" s="32"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
       <c r="E23" s="8" t="s">
         <v>11</v>
       </c>
@@ -3396,13 +3433,13 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="36" t="s">
+      <c r="A25" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="36" t="s">
+      <c r="C25" s="32" t="s">
         <v>138</v>
       </c>
       <c r="D25" s="8" t="s">
@@ -3413,10 +3450,10 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="36"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36" t="s">
+      <c r="A26" s="32"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32" t="s">
         <v>4</v>
       </c>
       <c r="E26" s="8" t="s">
@@ -3424,67 +3461,67 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="36"/>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
+      <c r="A27" s="32"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
       <c r="E27" s="8" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="36"/>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
+      <c r="A28" s="32"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
       <c r="E28" s="8" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="36"/>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
+      <c r="A29" s="32"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
       <c r="E29" s="8" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="36"/>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
+      <c r="A30" s="32"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
       <c r="E30" s="8" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="36"/>
-      <c r="B31" s="36"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="36"/>
+      <c r="A31" s="32"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
       <c r="E31" s="8" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="36"/>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
+      <c r="A32" s="32"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
       <c r="E32" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="36" t="s">
+      <c r="A33" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="B33" s="36" t="s">
+      <c r="B33" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C33" s="36" t="s">
+      <c r="C33" s="32" t="s">
         <v>143</v>
       </c>
       <c r="D33" s="8" t="s">
@@ -3495,10 +3532,10 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="36"/>
-      <c r="B34" s="36"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36" t="s">
+      <c r="A34" s="32"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32" t="s">
         <v>4</v>
       </c>
       <c r="E34" s="8" t="s">
@@ -3506,76 +3543,76 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="36"/>
-      <c r="B35" s="36"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="36"/>
+      <c r="A35" s="32"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
       <c r="E35" s="8" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="36"/>
-      <c r="B36" s="36"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
+      <c r="A36" s="32"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
       <c r="E36" s="8" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="36"/>
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
+      <c r="A37" s="32"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
       <c r="E37" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="36"/>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
+      <c r="A38" s="32"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
       <c r="E38" s="8" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="36"/>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
+      <c r="A39" s="32"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
       <c r="E39" s="8" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="36"/>
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
+      <c r="A40" s="32"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
       <c r="E40" s="8" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="36"/>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
+      <c r="A41" s="32"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
       <c r="E41" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="36" t="s">
+    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="32" t="s">
         <v>158</v>
       </c>
-      <c r="B42" s="36">
+      <c r="B42" s="32">
         <v>3</v>
       </c>
-      <c r="C42" s="36" t="s">
+      <c r="C42" s="32" t="s">
         <v>159</v>
       </c>
       <c r="D42" s="8" t="s">
@@ -3586,10 +3623,10 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36" t="s">
+      <c r="A43" s="32"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="32" t="s">
         <v>4</v>
       </c>
       <c r="E43" s="8" t="s">
@@ -3597,65 +3634,78 @@
       </c>
     </row>
     <row r="44" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
+      <c r="A44" s="32"/>
+      <c r="B44" s="32"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="32"/>
       <c r="E44" s="8" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="36"/>
+      <c r="A45" s="32"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="32"/>
       <c r="E45" s="9" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="36"/>
-      <c r="B46" s="36"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="36"/>
+      <c r="A46" s="32"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
       <c r="E46" s="8" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="36"/>
-      <c r="B47" s="36"/>
-      <c r="C47" s="36"/>
-      <c r="D47" s="36"/>
+      <c r="A47" s="32"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
       <c r="E47" s="9" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="36"/>
-      <c r="B48" s="36"/>
-      <c r="C48" s="36"/>
-      <c r="D48" s="36"/>
+      <c r="A48" s="32"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="32"/>
       <c r="E48" s="9" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="36"/>
-      <c r="B49" s="36"/>
-      <c r="C49" s="36"/>
-      <c r="D49" s="36"/>
+      <c r="A49" s="32"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
       <c r="E49" s="9" t="s">
         <v>136</v>
       </c>
     </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="32"/>
+      <c r="B50" s="32"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="D43:D49"/>
-    <mergeCell ref="C42:C49"/>
-    <mergeCell ref="B42:B49"/>
-    <mergeCell ref="A42:A49"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="C2:C13"/>
+    <mergeCell ref="D3:D13"/>
+    <mergeCell ref="A14:A23"/>
+    <mergeCell ref="B14:B23"/>
+    <mergeCell ref="C14:C23"/>
+    <mergeCell ref="D15:D23"/>
     <mergeCell ref="A25:A32"/>
     <mergeCell ref="B25:B32"/>
     <mergeCell ref="C25:C32"/>
@@ -3664,14 +3714,10 @@
     <mergeCell ref="B33:B41"/>
     <mergeCell ref="C33:C41"/>
     <mergeCell ref="D34:D41"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="C2:C13"/>
-    <mergeCell ref="D3:D13"/>
-    <mergeCell ref="A14:A23"/>
-    <mergeCell ref="B14:B23"/>
-    <mergeCell ref="C14:C23"/>
-    <mergeCell ref="D15:D23"/>
+    <mergeCell ref="D43:D50"/>
+    <mergeCell ref="C42:C50"/>
+    <mergeCell ref="B42:B50"/>
+    <mergeCell ref="A42:A50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>